<commit_message>
Mise en forme du Kanban pour toutes les stories, Valeur et Use cases et tableau d'avancement
</commit_message>
<xml_diff>
--- a/ressources-externes/Livrables/Etat_davancement.xlsx
+++ b/ressources-externes/Livrables/Etat_davancement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Documents\_OpenClassrooms\Git\Projet3-Dev4U\ressources-externes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernard\Documents\_OpenClassrooms\Git\Projet3-Dev4U\ressources-externes\Livrables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{434773BD-FAF4-499F-9E1F-5B2FC050FD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC322CB1-B1FC-41C9-9345-01AF494FBC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="-16320" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-180" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>Page se connecter 1</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Kanban</t>
   </si>
   <si>
-    <t>A faire</t>
-  </si>
-  <si>
     <t>Fait</t>
   </si>
   <si>
@@ -82,12 +79,15 @@
   </si>
   <si>
     <t>fait</t>
+  </si>
+  <si>
+    <t>Valeur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,19 +438,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -458,30 +458,36 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -492,13 +498,16 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -509,13 +518,16 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -526,135 +538,159 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
@@ -662,9 +698,12 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>